<commit_message>
Created figures and added them to presentation, expanded Implementation, and started writing Results section
</commit_message>
<xml_diff>
--- a/min_chi.xlsx
+++ b/min_chi.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="8055" tabRatio="986" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="8055" tabRatio="986" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="dt5_r100" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="4" r:id="rId2"/>
+    <sheet name="dt5_r10" sheetId="2" r:id="rId3"/>
+    <sheet name="Chart2" sheetId="5" r:id="rId4"/>
+    <sheet name="dt6_r100" sheetId="3" r:id="rId5"/>
+    <sheet name="Chart3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -108,110 +111,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-CH" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>dt = 1e-5 and </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>𝑟</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-CH" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t> ̃= 100</a:t>
-            </a:r>
-            <a:endParaRPr lang="de-CH">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18492436844882226"/>
+          <c:y val="5.2878482699206149E-2"/>
+          <c:w val="0.7735942546234218"/>
+          <c:h val="0.81941547068956422"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -226,15 +138,15 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -244,9 +156,9 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -256,8 +168,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.13500153105861767"/>
-                  <c:y val="0.12458333333333334"/>
+                  <c:x val="-0.1498014860818454"/>
+                  <c:y val="0.10463736822659507"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -273,7 +185,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -292,7 +204,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$6</c:f>
+              <c:f>dt5_r100!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -313,7 +225,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$6</c:f>
+              <c:f>dt5_r100!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -335,7 +247,239 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6489-4D51-926D-237A6A47770C}"/>
+              <c16:uniqueId val="{00000000-55D2-4AA0-8B31-068E67D6910C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>axis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{50209159-AD73-48B2-B571-BDC22A6E7E29}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-CH"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-55D2-4AA0-8B31-068E67D6910C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7BAC984B-4570-48DE-BDCA-BC717EFF8098}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-CH"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-55D2-4AA0-8B31-068E67D6910C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DA28B239-A84A-4666-9F7F-AD39961D0718}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-CH"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-55D2-4AA0-8B31-068E67D6910C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dt5_r100!$A$9:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dt5_r100!$B$9:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-55D2-4AA0-8B31-068E67D6910C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -354,23 +498,67 @@
         <c:axId val="401775072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="16"/>
+          <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH" sz="2000" b="1"/>
+                  <a:t>r</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -379,10 +567,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -393,11 +578,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
+                    <a:alpha val="0"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -419,32 +605,79 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="2000" b="1"/>
+                  <a:t>χ</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-CH" sz="2000" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6489534014857459E-2"/>
+              <c:y val="0.35646416995202312"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -455,7 +688,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -476,8 +709,10 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
-          <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -491,12 +726,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -511,11 +741,6 @@
       <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -533,110 +758,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-CH" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>dt = 1e-5 and </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>𝑟</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-CH" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t> ̃= 10</a:t>
-            </a:r>
-            <a:endParaRPr lang="de-CH">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18492436844882226"/>
+          <c:y val="5.2878482699206149E-2"/>
+          <c:w val="0.7735942546234218"/>
+          <c:h val="0.81941547068956422"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -651,15 +785,15 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -669,9 +803,9 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -681,8 +815,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.14055708661417324"/>
-                  <c:y val="0.1199537037037037"/>
+                  <c:x val="-0.1498014860818454"/>
+                  <c:y val="0.10463736822659507"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -698,7 +832,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -717,7 +851,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$3:$A$6</c:f>
+              <c:f>dt5_r10!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -738,7 +872,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$3:$B$6</c:f>
+              <c:f>dt5_r10!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -760,7 +894,238 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1E42-4F14-A7B2-5DCA83FE91B9}"/>
+              <c16:uniqueId val="{00000000-16B9-4878-8230-9747754AE15E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>axis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{50209159-AD73-48B2-B571-BDC22A6E7E29}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-CH"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-16B9-4878-8230-9747754AE15E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7BAC984B-4570-48DE-BDCA-BC717EFF8098}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-CH"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-16B9-4878-8230-9747754AE15E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DA28B239-A84A-4666-9F7F-AD39961D0718}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-CH"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-16B9-4878-8230-9747754AE15E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dt5_r100!$A$9:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dt5_r100!$B$9:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-16B9-4878-8230-9747754AE15E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -772,30 +1137,74 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="401779992"/>
-        <c:axId val="401775728"/>
+        <c:axId val="401775072"/>
+        <c:axId val="401775400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="401779992"/>
+        <c:axId val="401775072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="16"/>
+          <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH" sz="2000" b="1"/>
+                  <a:t>r</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -804,10 +1213,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -818,7 +1224,117 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                    <a:alpha val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="401775400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="401775400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="2000" b="1"/>
+                  <a:t>χ</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-CH" sz="2000" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6489534014857459E-2"/>
+              <c:y val="0.35646416995202312"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -833,76 +1349,16 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="401775728"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="401775728"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="401779992"/>
+        <c:crossAx val="401775072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
-          <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -916,12 +1372,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -936,11 +1387,6 @@
       <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -958,110 +1404,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-CH" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>dt = 1e-6 and </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>𝑟</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-CH" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t> ̃= 100</a:t>
-            </a:r>
-            <a:endParaRPr lang="de-CH">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19516764629773392"/>
+          <c:y val="5.2878482699206149E-2"/>
+          <c:w val="0.76335097677451014"/>
+          <c:h val="0.81941547068956422"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1076,15 +1431,15 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -1094,9 +1449,9 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
+                <a:prstDash val="sysDash"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1106,8 +1461,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.31227274715660541"/>
-                  <c:y val="0.37241652085156024"/>
+                  <c:x val="-0.11512839384193486"/>
+                  <c:y val="0.10498399765842797"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1123,7 +1478,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -1142,7 +1497,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$3:$A$6</c:f>
+              <c:f>dt6_r100!$A$3:$A$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1163,7 +1518,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$B$3:$B$6</c:f>
+              <c:f>dt6_r100!$B$3:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1185,7 +1540,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-212C-44A5-9E32-D637FB97AEA9}"/>
+              <c16:uniqueId val="{00000000-F5A1-42BA-9795-2CBFDE079783}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1193,7 +1548,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>series2</c:v>
+            <c:v>axis</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1203,83 +1558,210 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="plus"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{50209159-AD73-48B2-B571-BDC22A6E7E29}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-CH"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-F5A1-42BA-9795-2CBFDE079783}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7BAC984B-4570-48DE-BDCA-BC717EFF8098}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-CH"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-F5A1-42BA-9795-2CBFDE079783}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DA28B239-A84A-4666-9F7F-AD39961D0718}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="de-CH"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-F5A1-42BA-9795-2CBFDE079783}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="9.3282808398950132E-2"/>
-                  <c:y val="0.284060950714494"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$4:$A$6</c:f>
+              <c:f>dt6_r100!$A$9:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1287,18 +1769,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$B$4:$B$6</c:f>
+              <c:f>dt6_r100!$B$9:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>354000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>745000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1378500</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1306,7 +1803,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-212C-44A5-9E32-D637FB97AEA9}"/>
+              <c16:uniqueId val="{00000004-F5A1-42BA-9795-2CBFDE079783}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1318,30 +1815,74 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="478825904"/>
-        <c:axId val="478824592"/>
+        <c:axId val="401775072"/>
+        <c:axId val="401775400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="478825904"/>
+        <c:axId val="401775072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="105"/>
+          <c:min val="25"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH" sz="2000" b="1"/>
+                  <a:t>r</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1350,10 +1891,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1364,7 +1902,118 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                    <a:alpha val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="401775400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="401775400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="2000" b="1"/>
+                  <a:t>χ</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-CH" sz="2000" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6489534014857459E-2"/>
+              <c:y val="0.35646416995202312"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1379,77 +2028,16 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="478824592"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="478824592"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="478825904"/>
+        <c:crossAx val="401775072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
-          <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1463,12 +2051,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1483,11 +2066,6 @@
       <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -3159,25 +3737,53 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="11" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="11" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="11" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="7439025" cy="5210175"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3190,29 +3796,21 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>728662</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="7439025" cy="5210175"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3225,42 +3823,12 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>61912</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
@@ -3269,8 +3837,8 @@
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="102015" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -3306,6 +3874,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -3338,7 +3907,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -3394,6 +3963,33 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="7439025" cy="5210175"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3660,10 +4256,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3725,6 +4321,30 @@
         <v>221000</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3732,7 +4352,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3741,7 +4360,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3809,16 +4428,15 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3939,6 +4557,70 @@
         <v>1378500</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>70</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>80</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>90</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>100</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>

</xml_diff>

<commit_message>
Added conclusion to presentaion, modified min_chi plots, and continued Results section
</commit_message>
<xml_diff>
--- a/min_chi.xlsx
+++ b/min_chi.xlsx
@@ -118,9 +118,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18492436844882226"/>
+          <c:x val="0.23298844653764073"/>
           <c:y val="5.2878482699206149E-2"/>
-          <c:w val="0.7735942546234218"/>
+          <c:w val="0.72553010312963218"/>
           <c:h val="0.81941547068956422"/>
         </c:manualLayout>
       </c:layout>
@@ -421,7 +421,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -608,7 +607,7 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -625,10 +624,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="el-GR" sz="2000" b="1"/>
+                  <a:rPr lang="el-GR" sz="1800" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
                   <a:t>χ</a:t>
                 </a:r>
-                <a:endParaRPr lang="de-CH" sz="2000" b="1"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>min</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-CH" sz="2000">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -649,7 +658,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
@@ -765,9 +774,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18492436844882226"/>
+          <c:x val="0.23298844653764073"/>
           <c:y val="5.2878482699206149E-2"/>
-          <c:w val="0.7735942546234218"/>
+          <c:w val="0.72553010312963218"/>
           <c:h val="0.81941547068956422"/>
         </c:manualLayout>
       </c:layout>
@@ -1271,10 +1280,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="el-GR" sz="2000" b="1"/>
+                  <a:rPr lang="el-GR" sz="1800" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
                   <a:t>χ</a:t>
                 </a:r>
-                <a:endParaRPr lang="de-CH" sz="2000" b="1"/>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>min</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-CH" sz="2000">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1411,9 +1430,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.19516764629773392"/>
+          <c:x val="0.23255083768734516"/>
           <c:y val="5.2878482699206149E-2"/>
-          <c:w val="0.76335097677451014"/>
+          <c:w val="0.72596785214932247"/>
           <c:h val="0.81941547068956422"/>
         </c:manualLayout>
       </c:layout>
@@ -1952,6 +1971,10 @@
                 <a:r>
                   <a:rPr lang="el-GR" sz="2000" b="1"/>
                   <a:t>χ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" b="1" baseline="-25000"/>
+                  <a:t>min</a:t>
                 </a:r>
                 <a:endParaRPr lang="de-CH" sz="2000" b="1"/>
               </a:p>
@@ -3970,7 +3993,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="7439025" cy="5210175"/>
+    <xdr:ext cx="7134225" cy="4924425"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>

</xml_diff>

<commit_message>
cleaning up repository to move to GitHub
</commit_message>
<xml_diff>
--- a/min_chi.xlsx
+++ b/min_chi.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\infk\Linux\Documents\Seminar\repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samal\Documents\School\ETH\Courses\Term3\Seminar\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3B076E41-E10B-4F51-A2FE-817619E6273D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="8055" tabRatio="986" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17892" windowHeight="8052" tabRatio="986" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dt5_r100" sheetId="1" r:id="rId1"/>
@@ -18,6 +19,8 @@
     <sheet name="Chart2" sheetId="5" r:id="rId4"/>
     <sheet name="dt6_r100" sheetId="3" r:id="rId5"/>
     <sheet name="Chart3" sheetId="6" r:id="rId6"/>
+    <sheet name="Chart1_2" sheetId="7" r:id="rId7"/>
+    <sheet name="Chart3 (2)" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -197,7 +200,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -280,7 +283,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -291,7 +293,7 @@
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="de-CH"/>
+                    <a:endParaRPr lang="en-CA"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -304,7 +306,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -315,7 +316,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -326,7 +326,7 @@
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="de-CH"/>
+                    <a:endParaRPr lang="en-CA"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -339,7 +339,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -350,7 +349,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -361,7 +359,7 @@
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="de-CH"/>
+                    <a:endParaRPr lang="en-CA"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -374,7 +372,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -409,7 +406,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -528,7 +525,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -554,7 +550,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -590,7 +586,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="401775400"/>
@@ -674,7 +670,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -709,7 +705,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="401775072"/>
@@ -747,7 +743,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -853,7 +849,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -936,7 +932,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -947,7 +942,7 @@
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="de-CH"/>
+                    <a:endParaRPr lang="en-CA"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -960,7 +955,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -971,7 +965,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -982,7 +975,7 @@
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="de-CH"/>
+                    <a:endParaRPr lang="en-CA"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -995,7 +988,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -1006,7 +998,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -1017,7 +1008,7 @@
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="de-CH"/>
+                    <a:endParaRPr lang="en-CA"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1030,7 +1021,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -1065,7 +1055,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1184,7 +1174,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1210,7 +1199,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1246,7 +1235,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="401775400"/>
@@ -1330,7 +1319,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1365,7 +1354,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="401775072"/>
@@ -1403,7 +1392,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1509,7 +1498,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1592,7 +1581,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -1603,7 +1591,7 @@
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="de-CH"/>
+                    <a:endParaRPr lang="en-CA"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1616,7 +1604,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -1627,7 +1614,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -1638,7 +1624,7 @@
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="de-CH"/>
+                    <a:endParaRPr lang="en-CA"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1651,7 +1637,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -1662,7 +1647,6 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -1673,7 +1657,7 @@
                       <a:pPr/>
                       <a:t>[X VALUE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="de-CH"/>
+                    <a:endParaRPr lang="en-CA"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1686,7 +1670,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -1721,7 +1704,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="b"/>
@@ -1734,7 +1717,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1872,7 +1854,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1898,7 +1879,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1934,7 +1915,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="401775400"/>
@@ -2013,7 +1994,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2048,7 +2029,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="401775072"/>
@@ -2086,9 +2067,1451 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21074336960446682"/>
+          <c:y val="5.2878482699206149E-2"/>
+          <c:w val="0.74777509202520098"/>
+          <c:h val="0.81941547068956422"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.9295138159064819E-2"/>
+                  <c:y val="0.29463323663489432"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dt5_r100!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dt5_r100!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>114000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>221000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3582-445D-BB45-0B7722408D0B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>axis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{50209159-AD73-48B2-B571-BDC22A6E7E29}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-CA"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-3582-445D-BB45-0B7722408D0B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7BAC984B-4570-48DE-BDCA-BC717EFF8098}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-CA"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-3582-445D-BB45-0B7722408D0B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DA28B239-A84A-4666-9F7F-AD39961D0718}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-CA"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-3582-445D-BB45-0B7722408D0B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dt5_r100!$A$9:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dt5_r100!$B$9:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3582-445D-BB45-0B7722408D0B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>series2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="12700" cap="rnd">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.14353169277864902"/>
+                  <c:y val="0.14052470414882351"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dt5_r10!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dt5_r10!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>227000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-3582-445D-BB45-0B7722408D0B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="401775072"/>
+        <c:axId val="401775400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="401775072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH" sz="2000" b="1"/>
+                  <a:t>r</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                    <a:alpha val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="401775400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="401775400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1800" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>χ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>min</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-CH" sz="2000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6489534014857459E-2"/>
+              <c:y val="0.35646416995202312"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="401775072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.23255083768734516"/>
+          <c:y val="5.2878482699206149E-2"/>
+          <c:w val="0.72596785214932247"/>
+          <c:h val="0.81941547068956422"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.3510808582192112E-2"/>
+                  <c:y val="0.27303936240426085"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dt6_r100!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dt6_r100!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>31500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>354000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>745000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1378500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1925-4260-A9FB-F99985B7C3E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>axis</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{50209159-AD73-48B2-B571-BDC22A6E7E29}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-CA"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-1925-4260-A9FB-F99985B7C3E3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7BAC984B-4570-48DE-BDCA-BC717EFF8098}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-CA"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-1925-4260-A9FB-F99985B7C3E3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DA28B239-A84A-4666-9F7F-AD39961D0718}" type="XVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[X VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-CA"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="b"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-1925-4260-A9FB-F99985B7C3E3}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>dt6_r100!$A$9:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>dt6_r100!$B$9:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-1925-4260-A9FB-F99985B7C3E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="401775072"/>
+        <c:axId val="401775400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="401775072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="105"/>
+          <c:min val="25"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH" sz="2000" b="1"/>
+                  <a:t>r</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                    <a:alpha val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="401775400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="401775400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="2000" b="1"/>
+                  <a:t>χ</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" b="1" baseline="-25000"/>
+                  <a:t>min</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-CH" sz="2000" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6489534014857459E-2"/>
+              <c:y val="0.35646416995202312"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="401775072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2212,6 +3635,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3760,8 +5263,1040 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3773,7 +6308,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3785,10 +6320,34 @@
 </file>
 
 <file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="11" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{757875BA-7BC7-4A88-8621-60C893E931BD}">
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="11" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{AA1001A5-81F2-426A-9B4E-8DDCD34F5C4B}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="11" orientation="landscape" r:id="rId1"/>
@@ -3800,10 +6359,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="7439025" cy="5210175"/>
+    <xdr:ext cx="7421880" cy="5212080"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
@@ -3827,10 +6392,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="7439025" cy="5210175"/>
+    <xdr:ext cx="7421880" cy="5212080"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
@@ -3864,7 +6435,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="TextBox 2"/>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -3993,10 +6570,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="7134225" cy="4924425"/>
+    <xdr:ext cx="7421880" cy="5212080"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
@@ -4014,6 +6597,271 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="7421880" cy="5204460"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C10CEF5F-5685-43BE-89F8-412CD838F911}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.5616</cdr:x>
+      <cdr:y>0.17251</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.6848</cdr:x>
+      <cdr:y>0.23977</cdr:y>
+    </cdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <cdr:sp macro="" textlink="">
+          <cdr:nvSpPr>
+            <cdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98BE6866-4C25-4E45-8DA0-B8221EEF178C}"/>
+                </a:ext>
+              </a:extLst>
+            </cdr:cNvPr>
+            <cdr:cNvSpPr txBox="1"/>
+          </cdr:nvSpPr>
+          <cdr:spPr>
+            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:off x="4168140" y="899160"/>
+              <a:ext cx="914400" cy="350520"/>
+            </a:xfrm>
+            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </cdr:spPr>
+          <cdr:txBody>
+            <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+            <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+            <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:acc>
+                      <m:accPr>
+                        <m:chr m:val="̃"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-CA" sz="1800" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:accPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-CA" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑟</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:acc>
+                    <m:r>
+                      <a:rPr lang="en-CA" sz="1800" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=10</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-CA" sz="1800"/>
+            </a:p>
+          </cdr:txBody>
+        </cdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <cdr:sp macro="" textlink="">
+          <cdr:nvSpPr>
+            <cdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98BE6866-4C25-4E45-8DA0-B8221EEF178C}"/>
+                </a:ext>
+              </a:extLst>
+            </cdr:cNvPr>
+            <cdr:cNvSpPr txBox="1"/>
+          </cdr:nvSpPr>
+          <cdr:spPr>
+            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:off x="4168140" y="899160"/>
+              <a:ext cx="914400" cy="350520"/>
+            </a:xfrm>
+            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </cdr:spPr>
+          <cdr:txBody>
+            <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+            <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+            <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:r>
+                <a:rPr lang="en-CA" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑟 ̃=10</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-CA" sz="1800"/>
+            </a:p>
+          </cdr:txBody>
+        </cdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.74333</cdr:x>
+      <cdr:y>0.3538</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.86983</cdr:x>
+      <cdr:y>0.41112</cdr:y>
+    </cdr:to>
+    <cdr:pic>
+      <cdr:nvPicPr>
+        <cdr:cNvPr id="3" name="chart">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{771BBA56-2BDA-4CCF-8BDB-316842FFF53F}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cdr:cNvPicPr>
+      </cdr:nvPicPr>
+      <cdr:blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </cdr:blipFill>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5516880" y="1844040"/>
+          <a:ext cx="938865" cy="298730"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+    </cdr:pic>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="7421880" cy="5212080"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBBF6D88-7655-4D14-8FF7-2CAE302C8998}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76044</cdr:x>
+      <cdr:y>0.36209</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.88694</cdr:x>
+      <cdr:y>0.41932</cdr:y>
+    </cdr:to>
+    <cdr:pic>
+      <cdr:nvPicPr>
+        <cdr:cNvPr id="2" name="chart">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3DE800A-5F1B-4742-9ECF-70A99DA8C94A}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cdr:cNvPicPr>
+      </cdr:nvPicPr>
+      <cdr:blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </cdr:blipFill>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5643880" y="1887220"/>
+          <a:ext cx="938865" cy="298293"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+    </cdr:pic>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4278,19 +7126,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125"/>
+    <col min="1" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4304,7 +7152,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4312,7 +7160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -4320,7 +7168,7 @@
         <v>10500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -4328,7 +7176,7 @@
         <v>49500</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -4336,7 +7184,7 @@
         <v>114000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -4344,7 +7192,7 @@
         <v>221000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -4352,7 +7200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -4360,7 +7208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -4379,19 +7227,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125"/>
+    <col min="1" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4405,7 +7253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4413,7 +7261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -4421,7 +7269,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -4429,7 +7277,7 @@
         <v>51500</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -4437,7 +7285,7 @@
         <v>116500</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -4455,19 +7303,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125"/>
+    <col min="1" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4481,7 +7329,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4492,7 +7340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>30</v>
       </c>
@@ -4514,7 +7362,7 @@
         <v>31500</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -4536,7 +7384,7 @@
         <v>354000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>70</v>
       </c>
@@ -4558,7 +7406,7 @@
         <v>745000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>100</v>
       </c>
@@ -4580,7 +7428,7 @@
         <v>1378500</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
@@ -4588,7 +7436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -4596,7 +7444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>50</v>
       </c>
@@ -4604,7 +7452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>60</v>
       </c>
@@ -4612,7 +7460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>70</v>
       </c>
@@ -4620,7 +7468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>80</v>
       </c>
@@ -4628,7 +7476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>90</v>
       </c>
@@ -4636,7 +7484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>100</v>
       </c>

</xml_diff>